<commit_message>
Mise a jour des bureaux disponibles #8
</commit_message>
<xml_diff>
--- a/annexes/bureaux.xlsx
+++ b/annexes/bureaux.xlsx
@@ -24,9 +24,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Bureau</t>
   </si>
   <si>
@@ -66,10 +63,13 @@
     <t>O+361</t>
   </si>
   <si>
-    <t>+33748195</t>
-  </si>
-  <si>
     <t>bond@unice.fr</t>
+  </si>
+  <si>
+    <t>+336748195</t>
+  </si>
+  <si>
+    <t>Nom</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,16 +417,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -434,16 +434,16 @@
         <v>123456</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -451,16 +451,16 @@
         <v>123457</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -468,16 +468,16 @@
         <v>123458</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>